<commit_message>
Updated examples with recent API changes
</commit_message>
<xml_diff>
--- a/examples/data/example_data.xlsx
+++ b/examples/data/example_data.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">index</t>
   </si>
   <si>
-    <t xml:space="preserve">value (lcl=-2.5 ucl=2.5)</t>
+    <t xml:space="preserve">value (lsl=-2.5 usl=2.5)</t>
   </si>
 </sst>
 </file>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -128,7 +128,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.05"/>

</xml_diff>